<commit_message>
Add event study, late vs early compliers
</commit_message>
<xml_diff>
--- a/03_Tables/muestra_1porciento/SelfUpdate_twfe.xlsx
+++ b/03_Tables/muestra_1porciento/SelfUpdate_twfe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcomedina/ITAM Seira Research Dropbox/Marco Alejandro Medina/imss_rpci/03_Tables/muestra_1porciento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FECB45E-1A65-C647-9200-C186439161B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED2E871-9802-6C42-89E9-B9A607699750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16140" activeTab="1" xr2:uid="{5F2EF16D-A70A-3F40-9EFD-AA737EECFF16}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16140" activeTab="2" xr2:uid="{5F2EF16D-A70A-3F40-9EFD-AA737EECFF16}"/>
   </bookViews>
   <sheets>
     <sheet name="twfe_wage" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -157,9 +157,6 @@
     <t>Enrolled</t>
   </si>
   <si>
-    <t>Permanent Discharge</t>
-  </si>
-  <si>
     <t>Wage Change</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>Always Enrolled</t>
+  </si>
+  <si>
+    <t>Perm. Discharge</t>
   </si>
 </sst>
 </file>
@@ -337,7 +337,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -473,6 +473,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,18 +490,6 @@
     </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1315,23 +1312,23 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="twfe_cambio_cierre"/>
+      <sheetName val="twfe_sal_diff"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
         <row r="3">
-          <cell r="B3" t="str">
-            <v>0.004***</v>
+          <cell r="B3">
+            <v>2E-3</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>1E-3</v>
+            <v>2E-3</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>0.025***</v>
+            <v>0.327***</v>
           </cell>
         </row>
         <row r="6">
@@ -1346,7 +1343,7 @@
         </row>
         <row r="8">
           <cell r="B8">
-            <v>2.5000000000000001E-2</v>
+            <v>0.32700000000000001</v>
           </cell>
         </row>
         <row r="9">
@@ -1369,23 +1366,23 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="twfe_sal_diff"/>
+      <sheetName val="twfe_cambio_cierre"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
         <row r="3">
-          <cell r="B3">
-            <v>2E-3</v>
+          <cell r="B3" t="str">
+            <v>0.004***</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>2E-3</v>
+            <v>1E-3</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>0.327***</v>
+            <v>0.025***</v>
           </cell>
         </row>
         <row r="6">
@@ -1400,7 +1397,7 @@
         </row>
         <row r="8">
           <cell r="B8">
-            <v>0.32700000000000001</v>
+            <v>2.5000000000000001E-2</v>
           </cell>
         </row>
         <row r="9">
@@ -1824,18 +1821,18 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
@@ -1980,14 +1977,14 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
@@ -2404,16 +2401,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1FEA16-1BE8-3F4C-9FEA-B3431DB2F4D5}">
-  <dimension ref="B2:H16"/>
+  <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="B3:H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="B3:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="13.33203125" style="21" customWidth="1"/>
+    <col min="3" max="8" width="15" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2426,482 +2423,454 @@
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="53" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="37"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-    </row>
-    <row r="5" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+    <row r="4" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H4" s="25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="30" t="str" cm="1">
+        <f t="array" ref="C6:C9">[3]twfe_alta!$B$3:$B$6</f>
+        <v>0.050***</v>
+      </c>
+      <c r="D6" s="31" cm="1">
+        <f t="array" ref="D6:D9">[4]twfe_alta_cierre!$B$3:$B$6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E6" s="31" t="str" cm="1">
+        <f t="array" ref="E6:E9">[5]twfe_baja_cierre!$B$3:$B$6</f>
+        <v>0.011***</v>
+      </c>
+      <c r="F6" s="23" t="str" cm="1">
+        <f t="array" ref="F6:F9">[6]twfe_baja_permanente!$B$3:$B$6</f>
+        <v>0.010***</v>
+      </c>
+      <c r="G6" s="23" cm="1">
+        <f t="array" ref="G6:G9">[7]twfe_sal_diff!$B$3:$B$6</f>
+        <v>2E-3</v>
+      </c>
+      <c r="H6" s="23" t="str" cm="1">
+        <f t="array" ref="H6:H9">[8]twfe_cambio_cierre!$B$3:$B$6</f>
+        <v>0.004***</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="30" t="str" cm="1">
-        <f t="array" ref="C7:C10">[3]twfe_alta!$B$3:$B$6</f>
-        <v>0.050***</v>
-      </c>
-      <c r="D7" s="31" cm="1">
-        <f t="array" ref="D7:D10">[4]twfe_alta_cierre!$B$3:$B$6</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="26">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D7" s="27">
         <v>1E-3</v>
       </c>
-      <c r="E7" s="31" t="str" cm="1">
-        <f t="array" ref="E7:E10">[5]twfe_baja_cierre!$B$3:$B$6</f>
-        <v>0.011***</v>
-      </c>
-      <c r="F7" s="23" t="str" cm="1">
-        <f t="array" ref="F7:F10">[6]twfe_baja_permanente!$B$3:$B$6</f>
+      <c r="E7" s="27">
+        <v>1E-3</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
+        <v>2E-3</v>
+      </c>
+      <c r="H7" s="27">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="22" t="str">
+        <v>0.725***</v>
+      </c>
+      <c r="D8" s="23" t="str">
+        <v>0.025***</v>
+      </c>
+      <c r="E8" s="23" t="str">
+        <v>0.029***</v>
+      </c>
+      <c r="F8" s="23" t="str">
         <v>0.010***</v>
       </c>
-      <c r="G7" s="23" cm="1">
-        <f t="array" ref="G7:G10">[8]twfe_sal_diff!$B$3:$B$6</f>
-        <v>2E-3</v>
-      </c>
-      <c r="H7" s="23" t="str" cm="1">
-        <f t="array" ref="H7:H10">[7]twfe_cambio_cierre!$B$3:$B$6</f>
-        <v>0.004***</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="26">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D8" s="27">
-        <v>1E-3</v>
-      </c>
-      <c r="E8" s="27">
-        <v>1E-3</v>
-      </c>
-      <c r="F8" s="27">
-        <v>0</v>
-      </c>
-      <c r="G8" s="27">
-        <v>2E-3</v>
-      </c>
-      <c r="H8" s="27">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="G8" s="23" t="str">
+        <v>0.327***</v>
+      </c>
+      <c r="H8" s="23" t="str">
+        <v>0.025***</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="22" t="str">
-        <v>0.725***</v>
-      </c>
-      <c r="D9" s="23" t="str">
-        <v>0.025***</v>
-      </c>
-      <c r="E9" s="23" t="str">
-        <v>0.029***</v>
-      </c>
-      <c r="F9" s="23" t="str">
-        <v>0.010***</v>
-      </c>
-      <c r="G9" s="23" t="str">
-        <v>0.327***</v>
-      </c>
-      <c r="H9" s="23" t="str">
-        <v>0.025***</v>
+        <v>0</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27">
+        <v>0</v>
+      </c>
+      <c r="G9" s="27">
+        <v>0</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="26">
-        <v>0</v>
-      </c>
-      <c r="D10" s="27">
-        <v>0</v>
-      </c>
-      <c r="E10" s="27">
-        <v>0</v>
-      </c>
-      <c r="F10" s="27">
-        <v>0</v>
-      </c>
-      <c r="G10" s="27">
-        <v>0</v>
-      </c>
-      <c r="H10" s="27">
-        <v>0</v>
-      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="B11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="28" cm="1">
+        <f t="array" ref="C11:C14">[3]twfe_alta!$B$7:$B$10</f>
+        <v>8164128</v>
+      </c>
+      <c r="D11" s="29" cm="1">
+        <f t="array" ref="D11:D14">[4]twfe_alta_cierre!$B$7:$B$10</f>
+        <v>8164128</v>
+      </c>
+      <c r="E11" s="29" cm="1">
+        <f t="array" ref="E11:E14">[5]twfe_baja_cierre!$B$7:$B$10</f>
+        <v>8164128</v>
+      </c>
+      <c r="F11" s="29" cm="1">
+        <f t="array" ref="F11:F14">[6]twfe_baja_permanente!$B$7:$B$10</f>
+        <v>8164128</v>
+      </c>
+      <c r="G11" s="29" cm="1">
+        <f t="array" ref="G11:G14">[7]twfe_sal_diff!$B$7:$B$10</f>
+        <v>5645627</v>
+      </c>
+      <c r="H11" s="29" cm="1">
+        <f t="array" ref="H11:H14">[8]twfe_cambio_cierre!$B$7:$B$10</f>
+        <v>5645627</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="28" cm="1">
-        <f t="array" ref="C12:C15">[3]twfe_alta!$B$7:$B$10</f>
-        <v>8164128</v>
-      </c>
-      <c r="D12" s="29" cm="1">
-        <f t="array" ref="D12:D15">[4]twfe_alta_cierre!$B$7:$B$10</f>
-        <v>8164128</v>
-      </c>
-      <c r="E12" s="29" cm="1">
-        <f t="array" ref="E12:E15">[5]twfe_baja_cierre!$B$7:$B$10</f>
-        <v>8164128</v>
-      </c>
-      <c r="F12" s="29" cm="1">
-        <f t="array" ref="F12:F15">[6]twfe_baja_permanente!$B$7:$B$10</f>
-        <v>8164128</v>
-      </c>
-      <c r="G12" s="29" cm="1">
-        <f t="array" ref="G12:G15">[8]twfe_sal_diff!$B$7:$B$10</f>
-        <v>5645627</v>
-      </c>
-      <c r="H12" s="29" cm="1">
-        <f t="array" ref="H12:H15">[7]twfe_cambio_cierre!$B$7:$B$10</f>
-        <v>5645627</v>
+      <c r="B12" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="30">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D12" s="31">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E12" s="31">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F12" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="H12" s="31">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="30">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="D13" s="31">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E13" s="31">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F13" s="31">
-        <v>0.01</v>
-      </c>
-      <c r="G13" s="31">
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="H13" s="31">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C13" s="32">
         <v>255129</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D13" s="33">
         <v>255129</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E13" s="33">
         <v>255129</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F13" s="33">
         <v>255129</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G13" s="33">
         <v>242602</v>
       </c>
-      <c r="H14" s="33">
+      <c r="H13" s="33">
         <v>242602</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C14" s="34">
         <v>147147</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D14" s="35">
         <v>147147</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E14" s="35">
         <v>147147</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F14" s="35">
         <v>147147</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G14" s="35">
         <v>137124</v>
       </c>
-      <c r="H15" s="35">
+      <c r="H14" s="35">
         <v>137124</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB86A984-389A-2441-A526-FE946050D75F}">
-  <dimension ref="B2:E16"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="B3:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.33203125" customWidth="1"/>
+    <col min="3" max="5" width="22.5" style="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="2:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="2:5" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="E3" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="54" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="37"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="30" t="str" cm="1">
+        <f t="array" ref="C6:C9">[9]twfe_cambio_sal_mayor!$B$3:$B$6</f>
+        <v>0.002***</v>
+      </c>
+      <c r="D6" s="31" t="str" cm="1">
+        <f t="array" ref="D6:D9">[10]twfe_cambio_sal_menor!$B$3:$B$6</f>
+        <v>0.002***</v>
+      </c>
+      <c r="E6" s="31" cm="1">
+        <f t="array" ref="E6:E9">[11]twfe_cambio_sal_igual!$B$3:$B$6</f>
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="30" t="str" cm="1">
-        <f t="array" ref="C7:C10">[9]twfe_cambio_sal_mayor!$B$3:$B$6</f>
-        <v>0.002***</v>
-      </c>
-      <c r="D7" s="31" t="str" cm="1">
-        <f t="array" ref="D7:D10">[10]twfe_cambio_sal_menor!$B$3:$B$6</f>
-        <v>0.002***</v>
-      </c>
-      <c r="E7" s="31" cm="1">
-        <f t="array" ref="E7:E10">[11]twfe_cambio_sal_igual!$B$3:$B$6</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="26">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="27">
+        <v>1E-3</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="26">
-        <v>1E-3</v>
-      </c>
-      <c r="D8" s="27">
-        <v>1E-3</v>
-      </c>
-      <c r="E8" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="22" t="str">
+        <v>0.011***</v>
+      </c>
+      <c r="D8" s="23" t="str">
+        <v>0.009***</v>
+      </c>
+      <c r="E8" s="23" t="str">
+        <v>0.005***</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="22" t="str">
-        <v>0.011***</v>
-      </c>
-      <c r="D9" s="23" t="str">
-        <v>0.009***</v>
-      </c>
-      <c r="E9" s="23" t="str">
-        <v>0.005***</v>
+        <v>0</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="26">
-        <v>0</v>
-      </c>
-      <c r="D10" s="27">
-        <v>0</v>
-      </c>
-      <c r="E10" s="27">
-        <v>0</v>
-      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="28" cm="1">
+        <f t="array" ref="C11:C14">[9]twfe_cambio_sal_mayor!$B$7:$B$10</f>
+        <v>5645627</v>
+      </c>
+      <c r="D11" s="29" cm="1">
+        <f t="array" ref="D11:D14">[10]twfe_cambio_sal_menor!$B$7:$B$10</f>
+        <v>5645627</v>
+      </c>
+      <c r="E11" s="29" cm="1">
+        <f t="array" ref="E11:E14">[11]twfe_cambio_sal_igual!$B$7:$B$10</f>
+        <v>5645627</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="28" cm="1">
-        <f t="array" ref="C12:C15">[9]twfe_cambio_sal_mayor!$B$7:$B$10</f>
-        <v>5645627</v>
-      </c>
-      <c r="D12" s="29" cm="1">
-        <f t="array" ref="D12:D15">[10]twfe_cambio_sal_menor!$B$7:$B$10</f>
-        <v>5645627</v>
-      </c>
-      <c r="E12" s="29" cm="1">
-        <f t="array" ref="E12:E15">[11]twfe_cambio_sal_igual!$B$7:$B$10</f>
-        <v>5645627</v>
+      <c r="B12" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="30">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D12" s="31">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E12" s="31">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="30">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="D13" s="31">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="E13" s="31">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C13" s="32">
         <v>242602</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D13" s="33">
         <v>242602</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E13" s="33">
         <v>242602</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+    <row r="14" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C14" s="34">
         <v>137124</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D14" s="35">
         <v>137124</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E14" s="35">
         <v>137124</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="2:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2911,7 +2880,7 @@
   <dimension ref="B2:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="B3:D19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2933,10 +2902,10 @@
     <row r="3" spans="2:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="48"/>
       <c r="C3" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>32</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -2960,14 +2929,14 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
@@ -3054,10 +3023,10 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="53"/>
+      <c r="D11" s="56"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>

</xml_diff>